<commit_message>
write all codes to excel sheet
</commit_message>
<xml_diff>
--- a/naac.xlsx
+++ b/naac.xlsx
@@ -46,11 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -416,94 +413,130 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="18.2" customWidth="1" min="1" max="1"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n"/>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Classification</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CDC</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1.1.2</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CDC</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1.1.3</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CDC</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.3.2</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CDC</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1.3.4</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CDC</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1.4.1</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>TLEC</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2.1.2</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TLEC</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>2.4.3</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>INFRASTRUCTURE</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>3.1.3</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>3.3.2</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>3.3.3</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>3.4.3</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>3.4.5</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>3.4.6</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -511,36 +544,456 @@
       </c>
     </row>
     <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3.7.2</t>
+          <t>3.1.2</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DQAC</t>
+          <t>RESEARCH</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6.3.4</t>
+          <t>3.1.3</t>
         </is>
       </c>
       <c r="C10" t="n">
         <v>1</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>3.1.4</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>3.1.6</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>3.2.1</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>3.2.2</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>3.2.3</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>3.3.2</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>3.3.3</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3.4.3</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>3.4.4</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>3.4.5</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>3.4.6</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>3.4.7</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>3.5.2</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>3.6.2</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>RESEARCH</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>3.7.1</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>INFRASTRUCTURE</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>3.7.2</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>STUDENT SUPPORT</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>5.1.1</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>STUDENT SUPPORT</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>5.1.2</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>STUDENT SUPPORT</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>5.1.3</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>STUDENT SUPPORT</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>5.2.1</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>STUDENT SUPPORT</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>5.2.2</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>STUDENT SUPPORT</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>5.2.3</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>STUDENT SUPPORT</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>5.3.1</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>STUDENT SUPPORT</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>5.3.3</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>DQAC</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>6.3.2</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>DQAC</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>6.3.3</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>DQAC</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>6.3.4</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>DQAC</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>6.5.2</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A1"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Entering all spec codes
</commit_message>
<xml_diff>
--- a/naac.xlsx
+++ b/naac.xlsx
@@ -46,8 +46,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -420,9 +423,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Classification</t>
         </is>
@@ -439,7 +445,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>CDC</t>
         </is>
@@ -454,11 +460,6 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>CDC</t>
-        </is>
-      </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>1.1.3</t>
@@ -469,11 +470,6 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>CDC</t>
-        </is>
-      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>1.3.2</t>
@@ -484,11 +480,6 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>CDC</t>
-        </is>
-      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>1.3.4</t>
@@ -499,11 +490,6 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>CDC</t>
-        </is>
-      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>1.4.1</t>
@@ -514,7 +500,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>TLEC</t>
         </is>
@@ -529,11 +515,6 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>TLEC</t>
-        </is>
-      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>2.4.3</t>
@@ -544,7 +525,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>RESEARCH</t>
         </is>
@@ -559,11 +540,6 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>3.1.3</t>
@@ -574,11 +550,6 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>3.1.4</t>
@@ -589,11 +560,6 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B12" t="inlineStr">
         <is>
           <t>3.1.6</t>
@@ -604,11 +570,6 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B13" t="inlineStr">
         <is>
           <t>3.2.1</t>
@@ -619,11 +580,6 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>3.2.2</t>
@@ -634,11 +590,6 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B15" t="inlineStr">
         <is>
           <t>3.2.3</t>
@@ -649,11 +600,6 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B16" t="inlineStr">
         <is>
           <t>3.3.2</t>
@@ -664,11 +610,6 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B17" t="inlineStr">
         <is>
           <t>3.3.3</t>
@@ -679,11 +620,6 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B18" t="inlineStr">
         <is>
           <t>3.4.3</t>
@@ -694,11 +630,6 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B19" t="inlineStr">
         <is>
           <t>3.4.4</t>
@@ -709,11 +640,6 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B20" t="inlineStr">
         <is>
           <t>3.4.5</t>
@@ -724,11 +650,6 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B21" t="inlineStr">
         <is>
           <t>3.4.6</t>
@@ -739,11 +660,6 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B22" t="inlineStr">
         <is>
           <t>3.4.7</t>
@@ -754,11 +670,6 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B23" t="inlineStr">
         <is>
           <t>3.5.2</t>
@@ -769,11 +680,6 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B24" t="inlineStr">
         <is>
           <t>3.6.2</t>
@@ -784,11 +690,6 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>RESEARCH</t>
-        </is>
-      </c>
       <c r="B25" t="inlineStr">
         <is>
           <t>3.7.1</t>
@@ -799,7 +700,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="1" t="inlineStr">
         <is>
           <t>INFRASTRUCTURE</t>
         </is>
@@ -814,7 +715,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="1" t="inlineStr">
         <is>
           <t>STUDENT SUPPORT</t>
         </is>
@@ -829,11 +730,6 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>STUDENT SUPPORT</t>
-        </is>
-      </c>
       <c r="B28" t="inlineStr">
         <is>
           <t>5.1.2</t>
@@ -844,11 +740,6 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>STUDENT SUPPORT</t>
-        </is>
-      </c>
       <c r="B29" t="inlineStr">
         <is>
           <t>5.1.3</t>
@@ -859,11 +750,6 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>STUDENT SUPPORT</t>
-        </is>
-      </c>
       <c r="B30" t="inlineStr">
         <is>
           <t>5.2.1</t>
@@ -874,11 +760,6 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>STUDENT SUPPORT</t>
-        </is>
-      </c>
       <c r="B31" t="inlineStr">
         <is>
           <t>5.2.2</t>
@@ -889,11 +770,6 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>STUDENT SUPPORT</t>
-        </is>
-      </c>
       <c r="B32" t="inlineStr">
         <is>
           <t>5.2.3</t>
@@ -904,11 +780,6 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>STUDENT SUPPORT</t>
-        </is>
-      </c>
       <c r="B33" t="inlineStr">
         <is>
           <t>5.3.1</t>
@@ -919,11 +790,6 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>STUDENT SUPPORT</t>
-        </is>
-      </c>
       <c r="B34" t="inlineStr">
         <is>
           <t>5.3.3</t>
@@ -994,6 +860,14 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="A9:A25"/>
+    <mergeCell ref="A26"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
small error in gaps
</commit_message>
<xml_diff>
--- a/naac.xlsx
+++ b/naac.xlsx
@@ -17,13 +17,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +50,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -433,19 +440,19 @@
           <t>Classification</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Code</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>CDC</t>
         </is>
@@ -500,7 +507,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>TLEC</t>
         </is>
@@ -525,7 +532,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>RESEARCH</t>
         </is>
@@ -700,11 +707,6 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>INFRASTRUCTURE</t>
-        </is>
-      </c>
       <c r="B26" t="inlineStr">
         <is>
           <t>3.7.2</t>
@@ -715,7 +717,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
+      <c r="A27" s="2" t="inlineStr">
         <is>
           <t>STUDENT SUPPORT</t>
         </is>
@@ -800,7 +802,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="2" t="inlineStr">
         <is>
           <t>DQAC</t>
         </is>
@@ -815,11 +817,6 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>DQAC</t>
-        </is>
-      </c>
       <c r="B36" t="inlineStr">
         <is>
           <t>6.3.3</t>
@@ -830,11 +827,6 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>DQAC</t>
-        </is>
-      </c>
       <c r="B37" t="inlineStr">
         <is>
           <t>6.3.4</t>
@@ -845,11 +837,6 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>DQAC</t>
-        </is>
-      </c>
       <c r="B38" t="inlineStr">
         <is>
           <t>6.5.2</t>
@@ -861,11 +848,11 @@
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="A9:A25"/>
-    <mergeCell ref="A26"/>
+    <mergeCell ref="A9:A26"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A27:A34"/>
     <mergeCell ref="A1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>